<commit_message>
Manually apply changes to Orders spreadsheet
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Orders.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Orders.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimitarkokov/PycharmProjects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliot.smith/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECCCE9F7-561B-6143-8493-D47F361FE1B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009E09A3-B4A0-1F42-9945-31A6CF195C30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40960" yWindow="4720" windowWidth="25360" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36660" yWindow="660" windowWidth="35840" windowHeight="19900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="6" r:id="rId1"/>
@@ -24,11 +24,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">cases!$A$1:$Q$115</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -671,10 +666,10 @@
     <t>table_transforms</t>
   </si>
   <si>
+    <t>set_cases_orderstatus = {"source_cols": ["Ord Stat", "Ord Type"], "target_cols": ["orderstatus"]}</t>
+  </si>
+  <si>
     <t>mapped by table transform</t>
-  </si>
-  <si>
-    <t>set_cases_orderstatus = {"source_cols": ["Ord Stat", "Ord Type"], "target_cols": ["orderstatus"]}</t>
   </si>
 </sst>
 </file>
@@ -895,8 +890,8 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1111,11 +1106,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D9CE832-EC01-244E-8F8D-CFC70DCA6FD8}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1177,7 +1172,7 @@
         <v>210</v>
       </c>
       <c r="I2" s="30" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="29" customFormat="1">
@@ -1196,21 +1191,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C95" sqref="C95"/>
+      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I98" sqref="I98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -3513,7 +3503,7 @@
         <v>21</v>
       </c>
       <c r="Q95" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="96" spans="1:17" ht="15.75" customHeight="1">
@@ -5494,19 +5484,14 @@
     <row r="998" ht="13"/>
     <row r="999" ht="13"/>
   </sheetData>
-  <autoFilter ref="A1:Q115" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:Q115" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7067,16 +7052,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -8609,16 +8589,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -10121,22 +10096,17 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -11663,10 +11633,5 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>